<commit_message>
Update 5223002-2 Universal Pinout.xlsx
</commit_message>
<xml_diff>
--- a/2023/Backplane/Interconnect/5223002-2 Universal Pinout.xlsx
+++ b/2023/Backplane/Interconnect/5223002-2 Universal Pinout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\circu\Documents\Cal Poly Racing Baja\PCB\2023\Backplane\Interconnect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025298E6-4EC4-4138-BC12-8D460997035E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{687FB23A-3BE9-4ED4-92D4-F584796E692F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="26116" windowHeight="15675" xr2:uid="{C1EA6995-F0C0-4A93-A3BD-0B32422EA45A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>GND</t>
   </si>
@@ -196,12 +196,15 @@
   <si>
     <t>eCVT</t>
   </si>
+  <si>
+    <t>Product Page: https://www.te.com/usa-en/product-5223002-2.html</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -235,6 +238,14 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -358,10 +369,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -388,8 +400,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1193,28 +1207,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C166CB4-0D3E-452C-8525-B586843CFC7A}">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.8">
       <c r="A1" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
       <c r="B4" s="10" t="s">
         <v>36</v>
       </c>
@@ -1230,8 +1244,11 @@
       <c r="F4" s="10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="P4" s="24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1249,7 +1266,7 @@
       </c>
       <c r="F5" s="3"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1267,7 +1284,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1285,7 +1302,7 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1303,7 +1320,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1321,7 +1338,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1339,7 +1356,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1357,7 +1374,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1375,7 +1392,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1389,7 +1406,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1403,7 +1420,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1413,7 +1430,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1444,8 +1461,11 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="P4" r:id="rId1" xr:uid="{FDFBCE12-6D20-4288-9D07-169D17BFC884}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>